<commit_message>
Medidas .bdf en I mal,  ya modificadas
Solo las he modificados en lso archivos de iteracion. + El excell con algunas iteraciones
</commit_message>
<xml_diff>
--- a/Practica_2/BB/BB_Contol.xlsx
+++ b/Practica_2/BB/BB_Contol.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EUEP2\Git\EUE\Practica_2\BB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4008888F-C983-4DA0-969C-572B266F0FE9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF692E35-4A86-439A-AA5E-837A2E2A05DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FF95983B-251D-43E2-95FA-C41CB2890000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{FF95983B-251D-43E2-95FA-C41CB2890000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Rectangular" sheetId="1" r:id="rId1"/>
+    <sheet name="I" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="37">
   <si>
     <t>Material</t>
   </si>
@@ -45,9 +46,6 @@
     <t>Rigidizador exterior</t>
   </si>
   <si>
-    <t>Rigidizador interior</t>
-  </si>
-  <si>
     <t>Resultados</t>
   </si>
   <si>
@@ -118,6 +116,36 @@
   </si>
   <si>
     <t>Masa 2 [kg]</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>Rigidizador interior Rectangular</t>
+  </si>
+  <si>
+    <t>Rigidizador interior I</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>It2</t>
+  </si>
+  <si>
+    <t>It3</t>
+  </si>
+  <si>
+    <t>it4</t>
+  </si>
+  <si>
+    <t>it5</t>
+  </si>
+  <si>
+    <t>it6</t>
+  </si>
+  <si>
+    <t>Masa1</t>
   </si>
 </sst>
 </file>
@@ -382,6 +410,26 @@
   </cellStyleXfs>
   <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="8" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="9" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="9" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="9" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="12" xfId="9" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -390,9 +438,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -421,26 +466,9 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="8" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="5" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="6" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="7" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="7" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="9" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="9" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="9" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="12" xfId="9" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="20% - Énfasis1" xfId="3" builtinId="30"/>
@@ -764,10 +792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1DF7C73-B547-439B-A801-DFEA02B4BFAF}">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:W15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,102 +820,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4" t="s">
+      <c r="D1" s="20"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="8" t="s">
+      <c r="H1" s="23"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="13"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="30"/>
+      <c r="V1" t="s">
+        <v>36</v>
+      </c>
       <c r="W1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="C2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="17" t="s">
+      <c r="E2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="F2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="G2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="H2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="I2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="J2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="K2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="21" t="s">
+      <c r="Q2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="S2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="T2" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="U2" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="V2">
         <v>12</v>
-      </c>
-      <c r="N2" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="O2" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q2" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="R2" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="S2" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="T2" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="U2" s="24" t="s">
-        <v>19</v>
       </c>
       <c r="W2">
         <f>12*(2+3.5*0.46)</f>
@@ -895,19 +929,19 @@
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="26">
+      <c r="D3" s="13">
         <v>448000000</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="13">
         <v>523000000</v>
       </c>
       <c r="F3">
@@ -924,7 +958,7 @@
         <v>-7.4999999999999997E-3</v>
       </c>
       <c r="J3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K3">
         <v>5.0000000000000001E-3</v>
@@ -936,48 +970,42 @@
         <f>-(F3+L3)/2</f>
         <v>-7.4999999999999997E-3</v>
       </c>
-      <c r="N3" s="31">
+      <c r="N3" s="18">
         <v>57.971209999999999</v>
       </c>
-      <c r="O3" s="27">
+      <c r="O3" s="14">
         <f>N3-W2</f>
         <v>14.651209999999992</v>
       </c>
       <c r="P3">
-        <v>122.06</v>
-      </c>
-      <c r="Q3" s="26">
-        <v>104000000</v>
-      </c>
-      <c r="R3" s="26">
-        <v>414000000</v>
-      </c>
-      <c r="S3" s="26">
-        <v>21000000</v>
-      </c>
-      <c r="T3" s="27">
+        <v>49.88</v>
+      </c>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="13"/>
+      <c r="T3" s="14" t="e">
         <f xml:space="preserve"> D3/( MAX(Q3:S3)*1.1*1.2*1.1*1.25 ) - 1</f>
-        <v>-0.4037875460800362</v>
-      </c>
-      <c r="U3" s="27">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U3" s="14" t="e">
         <f xml:space="preserve"> E3/( MAX(Q3:S3)*1.1*1.2*1.1*1.25 ) - 1</f>
-        <v>-0.30397519330325651</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
+      <c r="A4" s="31" t="s">
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="26">
+        <v>20</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="13">
         <v>1000000000</v>
       </c>
-      <c r="E4" s="26">
+      <c r="E4" s="13">
         <v>1170000000</v>
       </c>
       <c r="F4">
@@ -994,7 +1022,7 @@
         <v>-7.4999999999999997E-3</v>
       </c>
       <c r="J4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K4">
         <v>5.0000000000000001E-3</v>
@@ -1006,27 +1034,736 @@
         <f>-(F4+L4)/2</f>
         <v>-7.4999999999999997E-3</v>
       </c>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="27">
-        <v>148.09710000000001</v>
-      </c>
-      <c r="Q4" s="26">
-        <v>109000000</v>
-      </c>
-      <c r="R4" s="26">
-        <v>437000000</v>
-      </c>
-      <c r="S4" s="26">
-        <v>22100000</v>
-      </c>
-      <c r="T4" s="27">
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="14">
+        <v>61.94</v>
+      </c>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="13"/>
+      <c r="S4" s="13"/>
+      <c r="T4" s="14" t="e">
         <f>D4/(MAX(Q4:S4)*1.1*1.2*1.1*1.25)-1</f>
-        <v>0.26078761402247985</v>
-      </c>
-      <c r="U4" s="27">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U4" s="14" t="e">
         <f xml:space="preserve"> E4/( MAX(Q4:S4)*1.1*1.2*1.1*1.25 ) - 1</f>
-        <v>0.47512150840630141</v>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="13">
+        <v>448000000</v>
+      </c>
+      <c r="E5" s="13">
+        <v>523000000</v>
+      </c>
+      <c r="F5">
+        <v>2E-3</v>
+      </c>
+      <c r="G5">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H5">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I5:I6" si="1">-(F5+H5)/2</f>
+        <v>-7.4999999999999997E-3</v>
+      </c>
+      <c r="J5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L5">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="M5">
+        <f>-(F5+L5)/2</f>
+        <v>-7.4999999999999997E-3</v>
+      </c>
+      <c r="N5" s="18"/>
+      <c r="O5" s="14"/>
+      <c r="P5">
+        <v>48.7</v>
+      </c>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="14" t="e">
+        <f xml:space="preserve"> D5/( MAX(Q5:S5)*1.1*1.2*1.1*1.25 ) - 1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U5" s="14" t="e">
+        <f xml:space="preserve"> E5/( MAX(Q5:S5)*1.1*1.2*1.1*1.25 ) - 1</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="13">
+        <v>1000000000</v>
+      </c>
+      <c r="E6" s="13">
+        <v>1170000000</v>
+      </c>
+      <c r="F6">
+        <v>2E-3</v>
+      </c>
+      <c r="G6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H6">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>-7.4999999999999997E-3</v>
+      </c>
+      <c r="J6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L6">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="M6">
+        <f>-(F6+L6)/2</f>
+        <v>-7.4999999999999997E-3</v>
+      </c>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="14">
+        <v>60.49</v>
+      </c>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="14" t="e">
+        <f>D6/(MAX(Q6:S6)*1.1*1.2*1.1*1.25)-1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U6" s="14" t="e">
+        <f xml:space="preserve"> E6/( MAX(Q6:S6)*1.1*1.2*1.1*1.25 ) - 1</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="13">
+        <v>1000000000</v>
+      </c>
+      <c r="E11" s="13">
+        <v>1170000000</v>
+      </c>
+      <c r="F11">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G11">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H11">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="I11">
+        <f t="shared" ref="I11" si="2">-(F11+H11)/2</f>
+        <v>-8.5000000000000006E-3</v>
+      </c>
+      <c r="J11" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L11">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="M11">
+        <f>-(F11+L11)/2</f>
+        <v>-8.5000000000000006E-3</v>
+      </c>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="14">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="13">
+        <v>1000000000</v>
+      </c>
+      <c r="E12" s="13">
+        <v>1170000000</v>
+      </c>
+      <c r="F12">
+        <v>2E-3</v>
+      </c>
+      <c r="G12">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H12">
+        <v>0.02</v>
+      </c>
+      <c r="I12">
+        <f t="shared" ref="I12" si="3">-(F12+H12)/2</f>
+        <v>-1.0999999999999999E-2</v>
+      </c>
+      <c r="J12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L12">
+        <v>0.02</v>
+      </c>
+      <c r="M12">
+        <f>-(F12+L12)/2</f>
+        <v>-1.0999999999999999E-2</v>
+      </c>
+      <c r="P12">
+        <v>94.35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="13">
+        <v>1000000000</v>
+      </c>
+      <c r="E13" s="13">
+        <v>1170000000</v>
+      </c>
+      <c r="F13">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G13">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H13">
+        <v>0.02</v>
+      </c>
+      <c r="I13">
+        <f t="shared" ref="I13" si="4">-(F13+H13)/2</f>
+        <v>-1.2E-2</v>
+      </c>
+      <c r="J13" t="s">
+        <v>22</v>
+      </c>
+      <c r="K13">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L13">
+        <v>0.02</v>
+      </c>
+      <c r="M13">
+        <f>-(F13+L13)/2</f>
+        <v>-1.2E-2</v>
+      </c>
+      <c r="P13">
+        <v>110.86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="13">
+        <v>1000000000</v>
+      </c>
+      <c r="E14" s="13">
+        <v>1170000000</v>
+      </c>
+      <c r="F14">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G14">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H14">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I14">
+        <f t="shared" ref="I14" si="5">-(F14+H14)/2</f>
+        <v>-1.4500000000000001E-2</v>
+      </c>
+      <c r="J14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L14">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="M14">
+        <f>-(F14+L14)/2</f>
+        <v>-1.4500000000000001E-2</v>
+      </c>
+      <c r="P14">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="13">
+        <v>1000000000</v>
+      </c>
+      <c r="E15" s="13">
+        <v>1170000000</v>
+      </c>
+      <c r="F15">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="G15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H15">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I15">
+        <f t="shared" ref="I15" si="6">-(F15+H15)/2</f>
+        <v>-1.55E-2</v>
+      </c>
+      <c r="J15" t="s">
+        <v>22</v>
+      </c>
+      <c r="K15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L15">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="M15">
+        <f>-(F15+L15)/2</f>
+        <v>-1.55E-2</v>
+      </c>
+      <c r="N15">
+        <v>63</v>
+      </c>
+      <c r="O15">
+        <f>N15-V2-W2</f>
+        <v>7.6799999999999926</v>
+      </c>
+      <c r="P15">
+        <v>150.91</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:U1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15ABF7DB-62C1-4981-A1EF-0E30BED6EA96}">
+  <dimension ref="A1:U6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="20"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="23"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="30"/>
+    </row>
+    <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="S2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="T2" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="U2" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="13">
+        <v>448000000</v>
+      </c>
+      <c r="E3" s="13">
+        <v>523000000</v>
+      </c>
+      <c r="F3">
+        <v>2E-3</v>
+      </c>
+      <c r="G3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H3">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I6" si="0">-(F3+H3)/2</f>
+        <v>-7.4999999999999997E-3</v>
+      </c>
+      <c r="J3">
+        <v>2E-3</v>
+      </c>
+      <c r="K3">
+        <v>0.01</v>
+      </c>
+      <c r="L3">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="M3">
+        <f>-(F3+L3)/2</f>
+        <v>-7.4999999999999997E-3</v>
+      </c>
+      <c r="N3" s="18">
+        <v>57.971209999999999</v>
+      </c>
+      <c r="O3" s="14">
+        <f>N3-W2</f>
+        <v>57.971209999999999</v>
+      </c>
+      <c r="P3">
+        <v>46.19</v>
+      </c>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="13"/>
+      <c r="T3" s="14" t="e">
+        <f xml:space="preserve"> D3/( MAX(Q3:S3)*1.1*1.2*1.1*1.25 ) - 1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U3" s="14" t="e">
+        <f xml:space="preserve"> E3/( MAX(Q3:S3)*1.1*1.2*1.1*1.25 ) - 1</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="13">
+        <v>1000000000</v>
+      </c>
+      <c r="E4" s="13">
+        <v>1170000000</v>
+      </c>
+      <c r="F4">
+        <v>2E-3</v>
+      </c>
+      <c r="G4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H4">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>-7.4999999999999997E-3</v>
+      </c>
+      <c r="J4">
+        <v>2E-3</v>
+      </c>
+      <c r="K4">
+        <v>0.01</v>
+      </c>
+      <c r="L4">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="M4">
+        <f>-(F4+L4)/2</f>
+        <v>-7.4999999999999997E-3</v>
+      </c>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="14">
+        <v>57.45</v>
+      </c>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="13"/>
+      <c r="S4" s="13"/>
+      <c r="T4" s="14" t="e">
+        <f>D4/(MAX(Q4:S4)*1.1*1.2*1.1*1.25)-1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U4" s="14" t="e">
+        <f xml:space="preserve"> E4/( MAX(Q4:S4)*1.1*1.2*1.1*1.25 ) - 1</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="13">
+        <v>448000000</v>
+      </c>
+      <c r="E5" s="13">
+        <v>523000000</v>
+      </c>
+      <c r="F5">
+        <v>2E-3</v>
+      </c>
+      <c r="G5">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H5">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>-7.4999999999999997E-3</v>
+      </c>
+      <c r="J5">
+        <v>2E-3</v>
+      </c>
+      <c r="K5">
+        <v>0.01</v>
+      </c>
+      <c r="L5">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="M5">
+        <f>-(F5+L5)/2</f>
+        <v>-7.4999999999999997E-3</v>
+      </c>
+      <c r="N5" s="18"/>
+      <c r="O5" s="14"/>
+      <c r="P5">
+        <v>47.27</v>
+      </c>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="14" t="e">
+        <f xml:space="preserve"> D5/( MAX(Q5:S5)*1.1*1.2*1.1*1.25 ) - 1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U5" s="14" t="e">
+        <f xml:space="preserve"> E5/( MAX(Q5:S5)*1.1*1.2*1.1*1.25 ) - 1</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="13">
+        <v>1000000000</v>
+      </c>
+      <c r="E6" s="13">
+        <v>1170000000</v>
+      </c>
+      <c r="F6">
+        <v>2E-3</v>
+      </c>
+      <c r="G6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H6">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>-7.4999999999999997E-3</v>
+      </c>
+      <c r="J6">
+        <v>2E-3</v>
+      </c>
+      <c r="K6">
+        <v>0.01</v>
+      </c>
+      <c r="L6">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="M6">
+        <f>-(F6+L6)/2</f>
+        <v>-7.4999999999999997E-3</v>
+      </c>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="14">
+        <v>58.77</v>
+      </c>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="14" t="e">
+        <f>D6/(MAX(Q6:S6)*1.1*1.2*1.1*1.25)-1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U6" s="14" t="e">
+        <f xml:space="preserve"> E6/( MAX(Q6:S6)*1.1*1.2*1.1*1.25 ) - 1</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>